<commit_message>
2019 12 06 21:25 inclusao das paginas de consulta
</commit_message>
<xml_diff>
--- a/testemunhoweb/logs/December.xlsx
+++ b/testemunhoweb/logs/December.xlsx
@@ -476,45 +476,45 @@
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t>Helaine Camilo</t>
+          <t>Jane</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr"/>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Graca</t>
         </is>
       </c>
       <c r="H4" s="4" t="inlineStr"/>
       <c r="I4" s="4" t="inlineStr"/>
       <c r="J4" s="4" t="inlineStr">
         <is>
-          <t>Icaro</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="K4" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Vinicius</t>
         </is>
       </c>
       <c r="L4" s="4" t="inlineStr">
         <is>
-          <t>Amintas</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="M4" s="4" t="inlineStr">
         <is>
-          <t>Dario</t>
+          <t>EMPTY</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>Cida</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr"/>
@@ -552,12 +552,12 @@
       <c r="I5" s="4" t="inlineStr"/>
       <c r="J5" s="4" t="inlineStr">
         <is>
-          <t>Icaro</t>
+          <t>Jessica Silva</t>
         </is>
       </c>
       <c r="K5" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Daiana</t>
         </is>
       </c>
       <c r="L5" s="4" t="inlineStr"/>
@@ -574,23 +574,23 @@
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>Ediane</t>
+          <t>Rodolfo Dias</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr"/>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>Robson</t>
+          <t>Lindoia</t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t>Patricia Dias</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="H6" s="4" t="inlineStr"/>
@@ -602,7 +602,7 @@
       </c>
       <c r="K6" s="4" t="inlineStr">
         <is>
-          <t>Vanda</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="L6" s="4" t="inlineStr"/>
@@ -624,7 +624,7 @@
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr"/>
@@ -648,12 +648,12 @@
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Robson</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>Daiana</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr"/>
@@ -664,29 +664,29 @@
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>Patricia Rodrigues</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr"/>
       <c r="I8" s="4" t="inlineStr"/>
       <c r="J8" s="4" t="inlineStr">
         <is>
-          <t>Beth</t>
+          <t>Vinicius</t>
         </is>
       </c>
       <c r="K8" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>EMPTY</t>
         </is>
       </c>
       <c r="L8" s="4" t="inlineStr">
         <is>
+          <t>Icaro</t>
+        </is>
+      </c>
+      <c r="M8" s="4" t="inlineStr">
+        <is>
           <t>Rodolfo Dias</t>
-        </is>
-      </c>
-      <c r="M8" s="4" t="inlineStr">
-        <is>
-          <t>Vinicius</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="K9" s="4" t="inlineStr">
         <is>
-          <t>Davi</t>
+          <t>Beth</t>
         </is>
       </c>
       <c r="L9" s="4" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="M9" s="4" t="inlineStr">
         <is>
-          <t>Icaro</t>
+          <t>Alex</t>
         </is>
       </c>
     </row>
@@ -753,18 +753,18 @@
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Helaine Camilo</t>
         </is>
       </c>
       <c r="D11" s="4" t="inlineStr">
         <is>
-          <t>Jane</t>
+          <t>Aline Lima</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr"/>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>Graca</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="G11" s="4" t="inlineStr">
@@ -776,22 +776,22 @@
       <c r="I11" s="4" t="inlineStr"/>
       <c r="J11" s="4" t="inlineStr">
         <is>
-          <t>Vinicius</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="K11" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="L11" s="4" t="inlineStr">
         <is>
-          <t>Marcio</t>
+          <t>Dario</t>
         </is>
       </c>
       <c r="M11" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Amintas</t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
       </c>
       <c r="D12" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Cida</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr"/>
@@ -822,19 +822,19 @@
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Patricia Rodrigues</t>
         </is>
       </c>
       <c r="H12" s="4" t="inlineStr"/>
       <c r="I12" s="4" t="inlineStr"/>
       <c r="J12" s="4" t="inlineStr">
         <is>
-          <t>Daiana</t>
+          <t>Icaro</t>
         </is>
       </c>
       <c r="K12" s="4" t="inlineStr">
         <is>
-          <t>Jessica Silva</t>
+          <t>Rodolfo Dias</t>
         </is>
       </c>
       <c r="L12" s="4" t="inlineStr"/>
@@ -856,13 +856,13 @@
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr"/>
       <c r="F13" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="G13" s="4" t="inlineStr">
@@ -874,12 +874,12 @@
       <c r="I13" s="4" t="inlineStr"/>
       <c r="J13" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="K13" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>EMPTY</t>
         </is>
       </c>
       <c r="L13" s="4" t="inlineStr"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="D14" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Lindoia</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr"/>
@@ -925,12 +925,12 @@
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
+          <t>Isabele</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
         <is>
-          <t>Eliane</t>
+          <t>Daiana</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr"/>
@@ -941,29 +941,29 @@
       </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Patricia Rodrigues</t>
         </is>
       </c>
       <c r="H15" s="4" t="inlineStr"/>
       <c r="I15" s="4" t="inlineStr"/>
       <c r="J15" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Beth</t>
         </is>
       </c>
       <c r="K15" s="4" t="inlineStr">
         <is>
+          <t>Aline Lima</t>
+        </is>
+      </c>
+      <c r="L15" s="4" t="inlineStr">
+        <is>
+          <t>Clayton</t>
+        </is>
+      </c>
+      <c r="M15" s="4" t="inlineStr">
+        <is>
           <t>EMPTY</t>
-        </is>
-      </c>
-      <c r="L15" s="4" t="inlineStr">
-        <is>
-          <t>Clayton</t>
-        </is>
-      </c>
-      <c r="M15" s="4" t="inlineStr">
-        <is>
-          <t>Icaro</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="K16" s="4" t="inlineStr">
         <is>
-          <t>Eliane</t>
+          <t>Carlos Eduardo</t>
         </is>
       </c>
       <c r="L16" s="4" t="inlineStr">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="M16" s="4" t="inlineStr">
         <is>
-          <t>Marcio</t>
+          <t>Douglas Oliveira</t>
         </is>
       </c>
     </row>
@@ -1030,40 +1030,40 @@
       </c>
       <c r="C18" s="4" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Jane</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr"/>
       <c r="F18" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Graca</t>
         </is>
       </c>
       <c r="G18" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="H18" s="4" t="inlineStr"/>
       <c r="I18" s="4" t="inlineStr"/>
       <c r="J18" s="4" t="inlineStr">
         <is>
-          <t>Helaine Camilo</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="K18" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="L18" s="4" t="inlineStr">
         <is>
-          <t>Dario</t>
+          <t>Marcio</t>
         </is>
       </c>
       <c r="M18" s="4" t="inlineStr">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="D19" s="4" t="inlineStr">
         <is>
-          <t>Vanda</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr"/>
@@ -1099,19 +1099,19 @@
       </c>
       <c r="G19" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="H19" s="4" t="inlineStr"/>
       <c r="I19" s="4" t="inlineStr"/>
       <c r="J19" s="4" t="inlineStr">
         <is>
-          <t>Icaro</t>
+          <t>Jessica Silva</t>
         </is>
       </c>
       <c r="K19" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Daiana</t>
         </is>
       </c>
       <c r="L19" s="4" t="inlineStr"/>
@@ -1133,30 +1133,30 @@
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Lindoia</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr"/>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Rodolfo Dias</t>
         </is>
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="H20" s="4" t="inlineStr"/>
       <c r="I20" s="4" t="inlineStr"/>
       <c r="J20" s="4" t="inlineStr">
         <is>
-          <t>Vanda</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="K20" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="L20" s="4" t="inlineStr"/>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
-          <t>Helaine Camilo</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr"/>
@@ -1202,12 +1202,12 @@
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>Daiana</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="E22" s="4" t="inlineStr"/>
@@ -1218,29 +1218,29 @@
       </c>
       <c r="G22" s="4" t="inlineStr">
         <is>
-          <t>Patricia Rodrigues</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="H22" s="4" t="inlineStr"/>
       <c r="I22" s="4" t="inlineStr"/>
       <c r="J22" s="4" t="inlineStr">
         <is>
-          <t>Beth</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="K22" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="L22" s="4" t="inlineStr">
         <is>
-          <t>Vinicius</t>
+          <t>Rodolfo Dias</t>
         </is>
       </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Icaro</t>
         </is>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="K23" s="4" t="inlineStr">
         <is>
-          <t>Davi</t>
+          <t>Marcio</t>
         </is>
       </c>
       <c r="L23" s="4" t="inlineStr">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>Telma</t>
+          <t>Icaro</t>
         </is>
       </c>
     </row>
@@ -1307,18 +1307,18 @@
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>Jane</t>
+          <t>Helaine Camilo</t>
         </is>
       </c>
       <c r="D25" s="4" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Aline Lima</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr"/>
       <c r="F25" s="4" t="inlineStr">
         <is>
-          <t>Graca</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="G25" s="4" t="inlineStr">
@@ -1330,22 +1330,22 @@
       <c r="I25" s="4" t="inlineStr"/>
       <c r="J25" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="K25" s="4" t="inlineStr">
         <is>
-          <t>Vinicius</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="L25" s="4" t="inlineStr">
         <is>
-          <t>Amintas</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="M25" s="4" t="inlineStr">
         <is>
-          <t>Marcio</t>
+          <t>EMPTY</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="D26" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="E26" s="4" t="inlineStr"/>
@@ -1383,12 +1383,12 @@
       <c r="I26" s="4" t="inlineStr"/>
       <c r="J26" s="4" t="inlineStr">
         <is>
-          <t>Jessica Silva</t>
+          <t>Icaro</t>
         </is>
       </c>
       <c r="K26" s="4" t="inlineStr">
         <is>
-          <t>Daiana</t>
+          <t>Rodolfo Dias</t>
         </is>
       </c>
       <c r="L26" s="4" t="inlineStr"/>
@@ -1405,30 +1405,30 @@
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>Ediane</t>
+          <t>Rodolfo Dias</t>
         </is>
       </c>
       <c r="D27" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Aline Lima</t>
         </is>
       </c>
       <c r="E27" s="4" t="inlineStr"/>
       <c r="F27" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="H27" s="4" t="inlineStr"/>
       <c r="I27" s="4" t="inlineStr"/>
       <c r="J27" s="4" t="inlineStr">
         <is>
-          <t>Patricia Dias</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="K27" s="4" t="inlineStr">
@@ -1479,12 +1479,12 @@
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Isabele</t>
         </is>
       </c>
       <c r="D29" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr"/>
@@ -1495,19 +1495,19 @@
       </c>
       <c r="G29" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Patricia Rodrigues</t>
         </is>
       </c>
       <c r="H29" s="4" t="inlineStr"/>
       <c r="I29" s="4" t="inlineStr"/>
       <c r="J29" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Aline Lima</t>
         </is>
       </c>
       <c r="K29" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="L29" s="4" t="inlineStr">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="M29" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Vinicius</t>
         </is>
       </c>
     </row>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="K30" s="4" t="inlineStr">
         <is>
-          <t>Karol</t>
+          <t>Alex</t>
         </is>
       </c>
       <c r="L30" s="4" t="inlineStr">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="M30" s="4" t="inlineStr">
         <is>
-          <t>Douglas Oliveira</t>
+          <t>Geronimo</t>
         </is>
       </c>
     </row>
@@ -1584,18 +1584,18 @@
       </c>
       <c r="C32" s="4" t="inlineStr">
         <is>
-          <t>Helaine Camilo</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="D32" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="E32" s="4" t="inlineStr"/>
       <c r="F32" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Graca</t>
         </is>
       </c>
       <c r="G32" s="4" t="inlineStr">
@@ -1607,22 +1607,22 @@
       <c r="I32" s="4" t="inlineStr"/>
       <c r="J32" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="K32" s="4" t="inlineStr">
         <is>
-          <t>Patricia Dias</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="L32" s="4" t="inlineStr">
         <is>
-          <t>Dario</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="M32" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Amintas</t>
         </is>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="D33" s="4" t="inlineStr">
         <is>
-          <t>Cida</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="E33" s="4" t="inlineStr"/>
@@ -1653,19 +1653,19 @@
       </c>
       <c r="G33" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
+          <t>Daiana</t>
         </is>
       </c>
       <c r="H33" s="4" t="inlineStr"/>
       <c r="I33" s="4" t="inlineStr"/>
       <c r="J33" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Jessica Silva</t>
         </is>
       </c>
       <c r="K33" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="L33" s="4" t="inlineStr"/>
@@ -1694,7 +1694,7 @@
       </c>
       <c r="B35" s="3" t="n"/>
       <c r="C35" s="5" t="n">
-        <v>43805.41836279045</v>
+        <v>43807.75785267639</v>
       </c>
       <c r="D35" s="4" t="n"/>
       <c r="E35" s="4" t="n"/>

</xml_diff>

<commit_message>
2019 12 19 inclusao do modulo histórico
</commit_message>
<xml_diff>
--- a/testemunhoweb/logs/December.xlsx
+++ b/testemunhoweb/logs/December.xlsx
@@ -380,7 +380,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,35 +476,35 @@
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
+          <t>Aline Lima</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
           <t>Jane</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Lucia</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr"/>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Graca</t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t>Graca</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="H4" s="4" t="inlineStr"/>
       <c r="I4" s="4" t="inlineStr"/>
       <c r="J4" s="4" t="inlineStr">
         <is>
+          <t>Vinicius</t>
+        </is>
+      </c>
+      <c r="K4" s="4" t="inlineStr">
+        <is>
           <t>Antonio</t>
-        </is>
-      </c>
-      <c r="K4" s="4" t="inlineStr">
-        <is>
-          <t>Vinicius</t>
         </is>
       </c>
       <c r="L4" s="4" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>Vanda</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr"/>
@@ -545,7 +545,7 @@
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
+          <t>Patricia Rodrigues</t>
         </is>
       </c>
       <c r="H5" s="4" t="inlineStr"/>
@@ -574,35 +574,35 @@
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Ediane</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr"/>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Conceicao</t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="H6" s="4" t="inlineStr"/>
       <c r="I6" s="4" t="inlineStr"/>
       <c r="J6" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Rodolfo</t>
         </is>
       </c>
       <c r="K6" s="4" t="inlineStr">
         <is>
-          <t>Patricia Dias</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="L6" s="4" t="inlineStr"/>
@@ -648,12 +648,12 @@
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>Robson</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Isabele</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr"/>
@@ -664,7 +664,7 @@
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr"/>
@@ -676,7 +676,7 @@
       </c>
       <c r="K8" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="L8" s="4" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="M8" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Clayton</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="K9" s="4" t="inlineStr">
         <is>
-          <t>Beth</t>
+          <t>Telma</t>
         </is>
       </c>
       <c r="L9" s="4" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="M9" s="4" t="inlineStr">
         <is>
-          <t>Alex</t>
+          <t>Douglas Oliveira</t>
         </is>
       </c>
     </row>
@@ -753,18 +753,18 @@
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
+          <t>Lucia</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
           <t>Helaine Camilo</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="inlineStr">
-        <is>
-          <t>Aline Lima</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr"/>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="G11" s="4" t="inlineStr">
@@ -776,17 +776,17 @@
       <c r="I11" s="4" t="inlineStr"/>
       <c r="J11" s="4" t="inlineStr">
         <is>
+          <t>Keila</t>
+        </is>
+      </c>
+      <c r="K11" s="4" t="inlineStr">
+        <is>
           <t>Valquiria</t>
         </is>
       </c>
-      <c r="K11" s="4" t="inlineStr">
-        <is>
-          <t>Patricia Dias</t>
-        </is>
-      </c>
       <c r="L11" s="4" t="inlineStr">
         <is>
-          <t>Dario</t>
+          <t>Marcio</t>
         </is>
       </c>
       <c r="M11" s="4" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="D12" s="4" t="inlineStr">
         <is>
-          <t>Cida</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr"/>
@@ -822,7 +822,7 @@
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>Patricia Rodrigues</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="H12" s="4" t="inlineStr"/>
@@ -834,7 +834,7 @@
       </c>
       <c r="K12" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Rodolfo</t>
         </is>
       </c>
       <c r="L12" s="4" t="inlineStr"/>
@@ -851,23 +851,23 @@
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
-          <t>Ediane</t>
+          <t>Rodolfo</t>
         </is>
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Robson</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr"/>
       <c r="F13" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Lindoia</t>
         </is>
       </c>
       <c r="G13" s="4" t="inlineStr">
         <is>
-          <t>Conceicao</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="H13" s="4" t="inlineStr"/>
@@ -879,7 +879,7 @@
       </c>
       <c r="K13" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="L13" s="4" t="inlineStr"/>
@@ -901,7 +901,7 @@
       </c>
       <c r="D14" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr"/>
@@ -925,12 +925,12 @@
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>Isabele</t>
+          <t>Daiana</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
         <is>
-          <t>Daiana</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr"/>
@@ -948,17 +948,17 @@
       <c r="I15" s="4" t="inlineStr"/>
       <c r="J15" s="4" t="inlineStr">
         <is>
-          <t>Beth</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="K15" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="L15" s="4" t="inlineStr">
         <is>
-          <t>Clayton</t>
+          <t>Rodolfo</t>
         </is>
       </c>
       <c r="M15" s="4" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="K16" s="4" t="inlineStr">
         <is>
-          <t>Carlos Eduardo</t>
+          <t>Alex</t>
         </is>
       </c>
       <c r="L16" s="4" t="inlineStr">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="M16" s="4" t="inlineStr">
         <is>
-          <t>Douglas Oliveira</t>
+          <t>Eliane</t>
         </is>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="C18" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="D18" s="4" t="inlineStr">
@@ -1041,34 +1041,34 @@
       <c r="E18" s="4" t="inlineStr"/>
       <c r="F18" s="4" t="inlineStr">
         <is>
+          <t>Aline Lima</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
           <t>Graca</t>
-        </is>
-      </c>
-      <c r="G18" s="4" t="inlineStr">
-        <is>
-          <t>Alana</t>
         </is>
       </c>
       <c r="H18" s="4" t="inlineStr"/>
       <c r="I18" s="4" t="inlineStr"/>
       <c r="J18" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
+          <t>Icaro</t>
         </is>
       </c>
       <c r="K18" s="4" t="inlineStr">
         <is>
-          <t>Eliane</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="L18" s="4" t="inlineStr">
         <is>
-          <t>Marcio</t>
+          <t>Dario</t>
         </is>
       </c>
       <c r="M18" s="4" t="inlineStr">
         <is>
-          <t>Icaro</t>
+          <t>EMPTY</t>
         </is>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="D19" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr"/>
@@ -1099,14 +1099,14 @@
       </c>
       <c r="G19" s="4" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="H19" s="4" t="inlineStr"/>
       <c r="I19" s="4" t="inlineStr"/>
       <c r="J19" s="4" t="inlineStr">
         <is>
-          <t>Jessica Silva</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="K19" s="4" t="inlineStr">
@@ -1133,30 +1133,30 @@
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Helaine Camilo</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr"/>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="H20" s="4" t="inlineStr"/>
       <c r="I20" s="4" t="inlineStr"/>
       <c r="J20" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="K20" s="4" t="inlineStr">
         <is>
-          <t>Patricia Dias</t>
+          <t>EMPTY</t>
         </is>
       </c>
       <c r="L20" s="4" t="inlineStr"/>
@@ -1225,17 +1225,17 @@
       <c r="I22" s="4" t="inlineStr"/>
       <c r="J22" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
+          <t>Aline Lima</t>
         </is>
       </c>
       <c r="K22" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Beth</t>
         </is>
       </c>
       <c r="L22" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Vinicius</t>
         </is>
       </c>
       <c r="M22" s="4" t="inlineStr">
@@ -1267,17 +1267,17 @@
       </c>
       <c r="K23" s="4" t="inlineStr">
         <is>
+          <t>Karol</t>
+        </is>
+      </c>
+      <c r="L23" s="4" t="inlineStr">
+        <is>
+          <t>Samuel</t>
+        </is>
+      </c>
+      <c r="M23" s="4" t="inlineStr">
+        <is>
           <t>Marcio</t>
-        </is>
-      </c>
-      <c r="L23" s="4" t="inlineStr">
-        <is>
-          <t>Samuel</t>
-        </is>
-      </c>
-      <c r="M23" s="4" t="inlineStr">
-        <is>
-          <t>Icaro</t>
         </is>
       </c>
     </row>
@@ -1312,13 +1312,13 @@
       </c>
       <c r="D25" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr"/>
       <c r="F25" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="G25" s="4" t="inlineStr">
@@ -1330,7 +1330,7 @@
       <c r="I25" s="4" t="inlineStr"/>
       <c r="J25" s="4" t="inlineStr">
         <is>
-          <t>Patricia Dias</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="K25" s="4" t="inlineStr">
@@ -1340,12 +1340,12 @@
       </c>
       <c r="L25" s="4" t="inlineStr">
         <is>
-          <t>Vanda</t>
+          <t>Amintas</t>
         </is>
       </c>
       <c r="M25" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Marcio</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="D26" s="4" t="inlineStr">
         <is>
-          <t>Vanda</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="E26" s="4" t="inlineStr"/>
@@ -1376,19 +1376,19 @@
       </c>
       <c r="G26" s="4" t="inlineStr">
         <is>
-          <t>Edith</t>
+          <t>Patricia Rodrigues</t>
         </is>
       </c>
       <c r="H26" s="4" t="inlineStr"/>
       <c r="I26" s="4" t="inlineStr"/>
       <c r="J26" s="4" t="inlineStr">
         <is>
-          <t>Icaro</t>
+          <t>Jessica Silva</t>
         </is>
       </c>
       <c r="K26" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>EMPTY</t>
         </is>
       </c>
       <c r="L26" s="4" t="inlineStr"/>
@@ -1405,23 +1405,23 @@
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Rodolfo</t>
         </is>
       </c>
       <c r="D27" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Lindoia</t>
         </is>
       </c>
       <c r="E27" s="4" t="inlineStr"/>
       <c r="F27" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="H27" s="4" t="inlineStr"/>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="D28" s="4" t="inlineStr">
         <is>
-          <t>Vinicius</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr"/>
@@ -1479,12 +1479,12 @@
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>Isabele</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="D29" s="4" t="inlineStr">
         <is>
-          <t>Eliane</t>
+          <t>Daiana</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr"/>
@@ -1495,29 +1495,29 @@
       </c>
       <c r="G29" s="4" t="inlineStr">
         <is>
-          <t>Patricia Rodrigues</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="H29" s="4" t="inlineStr"/>
       <c r="I29" s="4" t="inlineStr"/>
       <c r="J29" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="K29" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>EMPTY</t>
         </is>
       </c>
       <c r="L29" s="4" t="inlineStr">
         <is>
+          <t>Rodolfo</t>
+        </is>
+      </c>
+      <c r="M29" s="4" t="inlineStr">
+        <is>
           <t>Clayton</t>
-        </is>
-      </c>
-      <c r="M29" s="4" t="inlineStr">
-        <is>
-          <t>Vinicius</t>
         </is>
       </c>
     </row>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="K30" s="4" t="inlineStr">
         <is>
-          <t>Alex</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="L30" s="4" t="inlineStr">
@@ -1584,97 +1584,73 @@
       </c>
       <c r="C32" s="4" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="D32" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>EMPTY</t>
         </is>
       </c>
       <c r="E32" s="4" t="inlineStr"/>
       <c r="F32" s="4" t="inlineStr">
         <is>
-          <t>Graca</t>
+          <t>Aline Lima</t>
         </is>
       </c>
       <c r="G32" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="H32" s="4" t="inlineStr"/>
       <c r="I32" s="4" t="inlineStr"/>
       <c r="J32" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="K32" s="4" t="inlineStr">
         <is>
-          <t>Eliane</t>
+          <t>EMPTY</t>
         </is>
       </c>
       <c r="L32" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Dario</t>
         </is>
       </c>
       <c r="M32" s="4" t="inlineStr">
         <is>
-          <t>Amintas</t>
+          <t>Icaro</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" s="3" t="inlineStr">
-        <is>
-          <t>Terca-feira</t>
-        </is>
-      </c>
-      <c r="C33" s="4" t="inlineStr">
-        <is>
-          <t>Lindoia</t>
-        </is>
-      </c>
-      <c r="D33" s="4" t="inlineStr">
-        <is>
-          <t>Eliane</t>
-        </is>
-      </c>
-      <c r="E33" s="4" t="inlineStr"/>
-      <c r="F33" s="4" t="inlineStr">
-        <is>
-          <t>Luciana</t>
-        </is>
-      </c>
-      <c r="G33" s="4" t="inlineStr">
-        <is>
-          <t>Daiana</t>
-        </is>
-      </c>
-      <c r="H33" s="4" t="inlineStr"/>
-      <c r="I33" s="4" t="inlineStr"/>
-      <c r="J33" s="4" t="inlineStr">
-        <is>
-          <t>Jessica Silva</t>
-        </is>
-      </c>
-      <c r="K33" s="4" t="inlineStr">
-        <is>
-          <t>Alana</t>
-        </is>
-      </c>
-      <c r="L33" s="4" t="inlineStr"/>
-      <c r="M33" s="4" t="inlineStr"/>
+      <c r="A33" s="3" t="n"/>
+      <c r="B33" s="3" t="n"/>
+      <c r="C33" s="4" t="n"/>
+      <c r="D33" s="4" t="n"/>
+      <c r="E33" s="4" t="n"/>
+      <c r="F33" s="4" t="n"/>
+      <c r="G33" s="4" t="n"/>
+      <c r="H33" s="4" t="n"/>
+      <c r="I33" s="4" t="n"/>
+      <c r="J33" s="4" t="n"/>
+      <c r="K33" s="4" t="n"/>
+      <c r="L33" s="4" t="n"/>
+      <c r="M33" s="4" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="n"/>
+      <c r="A34" s="3" t="inlineStr">
+        <is>
+          <t>Data de geracao</t>
+        </is>
+      </c>
       <c r="B34" s="3" t="n"/>
-      <c r="C34" s="4" t="n"/>
+      <c r="C34" s="5" t="n">
+        <v>43818.59197647273</v>
+      </c>
       <c r="D34" s="4" t="n"/>
       <c r="E34" s="4" t="n"/>
       <c r="F34" s="4" t="n"/>
@@ -1687,15 +1663,9 @@
       <c r="M34" s="4" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="inlineStr">
-        <is>
-          <t>Data de geracao</t>
-        </is>
-      </c>
+      <c r="A35" s="3" t="n"/>
       <c r="B35" s="3" t="n"/>
-      <c r="C35" s="5" t="n">
-        <v>43807.75785267639</v>
-      </c>
+      <c r="C35" s="4" t="n"/>
       <c r="D35" s="4" t="n"/>
       <c r="E35" s="4" t="n"/>
       <c r="F35" s="4" t="n"/>
@@ -1722,25 +1692,10 @@
       <c r="L36" s="4" t="n"/>
       <c r="M36" s="4" t="n"/>
     </row>
-    <row r="37">
-      <c r="A37" s="3" t="n"/>
-      <c r="B37" s="3" t="n"/>
-      <c r="C37" s="4" t="n"/>
-      <c r="D37" s="4" t="n"/>
-      <c r="E37" s="4" t="n"/>
-      <c r="F37" s="4" t="n"/>
-      <c r="G37" s="4" t="n"/>
-      <c r="H37" s="4" t="n"/>
-      <c r="I37" s="4" t="n"/>
-      <c r="J37" s="4" t="n"/>
-      <c r="K37" s="4" t="n"/>
-      <c r="L37" s="4" t="n"/>
-      <c r="M37" s="4" t="n"/>
-    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:F34"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:G2"/>

</xml_diff>